<commit_message>
added all variables xlsx files for 2021/2022
</commit_message>
<xml_diff>
--- a/sui/data/checklist.xlsx
+++ b/sui/data/checklist.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="25">
   <si>
     <t>Variable</t>
   </si>
@@ -89,9 +89,6 @@
   </si>
   <si>
     <t>X</t>
-  </si>
-  <si>
-    <t>-</t>
   </si>
 </sst>
 </file>
@@ -516,7 +513,7 @@
   <dimension ref="B3:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -605,9 +602,11 @@
         <v>20</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="F7" s="15"/>
+        <v>24</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="8" spans="2:6" ht="45.2" x14ac:dyDescent="0.3">
       <c r="B8" s="12" t="s">
@@ -619,8 +618,12 @@
       <c r="D8" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
+      <c r="E8" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="9" spans="2:6" ht="30.15" x14ac:dyDescent="0.3">
       <c r="B9" s="6" t="s">

</xml_diff>